<commit_message>
cambios en Documentacion/Pruebas Noviembre/INCIDENCIAS.xlsx
</commit_message>
<xml_diff>
--- a/Documentacion/Pruebas Noviembre/INCIDENCIAS.xlsx
+++ b/Documentacion/Pruebas Noviembre/INCIDENCIAS.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ENTORNO_SGS\Fuentes\workspace\Documentacion\Pruebas Noviembre\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CLIENTES" sheetId="1" r:id="rId1"/>
     <sheet name="ASEGURADORA" sheetId="2" r:id="rId2"/>
     <sheet name="ACCPERSONALES" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="47">
   <si>
     <t xml:space="preserve">REPORTE DE INCIDENCIAS </t>
   </si>
@@ -143,12 +138,36 @@
   </si>
   <si>
     <t>Cuando grabo un contacto nuevo graba  en minusculas</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Solo deja ingresar 13 caracteres</t>
+  </si>
+  <si>
+    <t>Es campo no es obligatorio</t>
+  </si>
+  <si>
+    <t>Capturar pantalla para ver el error</t>
+  </si>
+  <si>
+    <t>La aseguradora es en la nueva que estoy agregando</t>
+  </si>
+  <si>
+    <t>Explicar de mejor manera</t>
+  </si>
+  <si>
+    <t>Esto no es de aseguradora</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,12 +193,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -244,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -274,6 +299,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -312,7 +353,7 @@
         <xdr:cNvPr id="2" name="Imagen 1" descr="C:\Users\kruger\Dropbox\JIPOVI\Documentos Varios\logoJipovi.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9F0756E-9FB8-4B54-B059-B9514945C028}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E9F0756E-9FB8-4B54-B059-B9514945C028}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -370,7 +411,7 @@
         <xdr:cNvPr id="2" name="Imagen 1" descr="C:\Users\kruger\Dropbox\JIPOVI\Documentos Varios\logoJipovi.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD4C2787-9CA9-46F8-B0D9-4BC4DDCBF2F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DD4C2787-9CA9-46F8-B0D9-4BC4DDCBF2F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -428,7 +469,7 @@
         <xdr:cNvPr id="2" name="Imagen 1" descr="C:\Users\kruger\Dropbox\JIPOVI\Documentos Varios\logoJipovi.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCC3D88E-A717-4C60-A463-537184D77F69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BCC3D88E-A717-4C60-A463-537184D77F69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -509,7 +550,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -561,7 +602,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -755,7 +796,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -763,25 +804,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A10:C31"/>
+  <dimension ref="A10:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>1</v>
       </c>
@@ -790,7 +832,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
         <v>3</v>
@@ -798,8 +840,11 @@
       <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -807,17 +852,21 @@
       <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -825,8 +874,9 @@
       <c r="C15" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>10</v>
       </c>
@@ -834,8 +884,9 @@
       <c r="C16" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
@@ -843,8 +894,9 @@
       <c r="C17" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>12</v>
       </c>
@@ -852,8 +904,9 @@
       <c r="C18" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
@@ -861,8 +914,9 @@
       <c r="C19" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
@@ -870,8 +924,9 @@
       <c r="C20" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>15</v>
       </c>
@@ -879,8 +934,9 @@
       <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -888,8 +944,9 @@
       <c r="C22" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>17</v>
       </c>
@@ -897,8 +954,9 @@
       <c r="C23" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>27</v>
       </c>
@@ -906,17 +964,19 @@
       <c r="C24" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>34</v>
       </c>
@@ -924,41 +984,49 @@
       <c r="C26" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="7"/>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="B27" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="B28" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -972,25 +1040,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A10:C35"/>
+  <dimension ref="A10:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
+    <col min="4" max="4" width="29" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>1</v>
       </c>
@@ -999,7 +1068,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
         <v>3</v>
@@ -1007,8 +1076,11 @@
       <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
@@ -1016,8 +1088,9 @@
       <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>18</v>
       </c>
@@ -1025,8 +1098,9 @@
         <v>8</v>
       </c>
       <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
@@ -1034,8 +1108,9 @@
       <c r="C15" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
@@ -1043,8 +1118,9 @@
       <c r="C16" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
@@ -1052,8 +1128,11 @@
         <v>8</v>
       </c>
       <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D17" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>22</v>
       </c>
@@ -1061,8 +1140,11 @@
         <v>8</v>
       </c>
       <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>23</v>
       </c>
@@ -1070,8 +1152,11 @@
         <v>8</v>
       </c>
       <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>24</v>
       </c>
@@ -1079,8 +1164,9 @@
         <v>8</v>
       </c>
       <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>25</v>
       </c>
@@ -1088,8 +1174,9 @@
       <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>26</v>
       </c>
@@ -1097,8 +1184,9 @@
       <c r="C22" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
@@ -1106,8 +1194,9 @@
         <v>8</v>
       </c>
       <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>30</v>
       </c>
@@ -1115,8 +1204,11 @@
         <v>8</v>
       </c>
       <c r="C24" s="7"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>33</v>
       </c>
@@ -1124,8 +1216,11 @@
         <v>8</v>
       </c>
       <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>38</v>
       </c>
@@ -1133,51 +1228,61 @@
       <c r="C26" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="9"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
+      <c r="D35" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1196,7 +1301,7 @@
       <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
   </cols>
@@ -1208,7 +1313,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>1</v>
       </c>
@@ -1217,7 +1322,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
         <v>3</v>
@@ -1226,7 +1331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
@@ -1235,7 +1340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>18</v>
       </c>
@@ -1253,7 +1358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
@@ -1262,7 +1367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
@@ -1280,7 +1385,7 @@
       </c>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>23</v>
       </c>
@@ -1289,7 +1394,7 @@
       </c>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>24</v>
       </c>
@@ -1298,7 +1403,7 @@
       </c>
       <c r="C20" s="7"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>25</v>
       </c>
@@ -1307,7 +1412,7 @@
       </c>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>26</v>
       </c>
@@ -1316,7 +1421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
@@ -1325,7 +1430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
@@ -1352,7 +1457,7 @@
       </c>
       <c r="C26" s="7"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>32</v>
       </c>
@@ -1361,7 +1466,7 @@
       </c>
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>33</v>
       </c>
@@ -1370,7 +1475,7 @@
       </c>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>34</v>
       </c>
@@ -1397,17 +1502,17 @@
       </c>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>

</xml_diff>